<commit_message>
pytest now works with bearer even when not in debug mode
</commit_message>
<xml_diff>
--- a/documentation/Automatic_tests.xlsx
+++ b/documentation/Automatic_tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7A93D1-C0F6-6A44-8315-E7E059C1AB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21A4ED1-CAAA-294A-8A94-042913606740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1100" windowWidth="23120" windowHeight="19300" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="89">
   <si>
     <t>-</t>
   </si>
@@ -280,9 +280,6 @@
     <t>Invalid login attempt. Please try again.</t>
   </si>
   <si>
-    <t>{"access_token": "*STRING", "token_type": "bearer"}</t>
-  </si>
-  <si>
     <t>Acknowledged</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>email, password</t>
+  </si>
+  <si>
+    <t>{"access_token": "*STRING", "token_type": "Bearer"}</t>
   </si>
 </sst>
 </file>
@@ -979,7 +979,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>6</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
@@ -1015,7 +1015,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="10">
         <v>80</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>6</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>6</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>6</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
@@ -1177,7 +1177,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E10" s="10">
         <v>10</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>6</v>
@@ -1207,7 +1207,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" s="10">
         <v>10</v>
@@ -1228,7 +1228,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>6</v>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>6</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>6</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>6</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>6</v>
@@ -1437,7 +1437,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1482,8 +1482,8 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2432,9 +2432,7 @@
       <c r="H23" s="28">
         <v>200</v>
       </c>
-      <c r="I23" s="16" t="s">
-        <v>80</v>
-      </c>
+      <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="26">
         <v>10</v>
@@ -2593,7 +2591,7 @@
         <v>200</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="J27" s="20"/>
       <c r="K27" s="29">

</xml_diff>

<commit_message>
Login password must be repeated
</commit_message>
<xml_diff>
--- a/documentation/Automatic_tests.xlsx
+++ b/documentation/Automatic_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8518C314-D79A-3B4A-9B6E-1F0EF6F4AAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F8266D-C501-2E46-BB37-BAB3916461DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1100" windowWidth="23120" windowHeight="19300" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="91">
   <si>
     <t>-</t>
   </si>
@@ -211,15 +211,9 @@
     <t>TC</t>
   </si>
   <si>
-    <t>{"email": "dummy@sample.com", "password": "Right-Password01!"}</t>
-  </si>
-  <si>
     <t>{"email": "dummy@sample.com", "password": "Right-Password1!", "new_password": "Right-New_Password1!",  "new_password_repeated": "Right-New_Password1!"}</t>
   </si>
   <si>
-    <t>{"email": "dummy@sample.com", "password": "Right-Password1!"}</t>
-  </si>
-  <si>
     <t>{"email": "dummy@sample.com", "password": "Wrong-Password!", "new_password": "Right-New_Password1!",  "new_password_repeated": "Right-New_Password1!"}</t>
   </si>
   <si>
@@ -305,6 +299,18 @@
   </si>
   <si>
     <t>Invalid login attempt.</t>
+  </si>
+  <si>
+    <t>{"email": "dummy@sample.com", "password": "Right-Password1!", "password_repeat": "Right-Password1!"}</t>
+  </si>
+  <si>
+    <t>{"email": "dummy@sample.com", "password": "Right-Password1!", "password_repeat": "Wrong-Password1!"}</t>
+  </si>
+  <si>
+    <t>{"email": "dummy@sample.com", "password": "Wrong-Password1!", "password_repeat": "Right-Password1!"}</t>
+  </si>
+  <si>
+    <t>Repeated password must be the same.</t>
   </si>
 </sst>
 </file>
@@ -979,7 +985,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>6</v>
@@ -1006,7 +1012,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>6</v>
@@ -1015,7 +1021,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E4" s="10">
         <v>80</v>
@@ -1033,7 +1039,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>6</v>
@@ -1060,7 +1066,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>6</v>
@@ -1090,7 +1096,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -1114,7 +1120,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
@@ -1139,12 +1145,12 @@
         <v>Acknowledged</v>
       </c>
       <c r="J8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>6</v>
@@ -1168,7 +1174,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
@@ -1177,7 +1183,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E10" s="10">
         <v>10</v>
@@ -1198,7 +1204,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>6</v>
@@ -1207,7 +1213,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E11" s="10">
         <v>10</v>
@@ -1228,7 +1234,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>6</v>
@@ -1252,7 +1258,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>6</v>
@@ -1282,7 +1288,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>6</v>
@@ -1312,7 +1318,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>6</v>
@@ -1336,7 +1342,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>6</v>
@@ -1437,7 +1443,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1479,11 +1485,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DB7162-4CDB-1E49-A9D6-A74F09DB89DA}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,7 +1517,7 @@
         <v>56</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
@@ -1522,12 +1528,12 @@
         <v>52</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
       <c r="K1" s="37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L1" s="36"/>
       <c r="M1" s="36"/>
@@ -1550,19 +1556,19 @@
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
       <c r="H2" s="38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J2" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="L2" s="38" t="s">
         <v>66</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>68</v>
       </c>
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
@@ -1591,10 +1597,10 @@
         <v>422</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K3" s="24">
         <v>99</v>
@@ -1610,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>45</v>
       </c>
@@ -1623,7 +1629,7 @@
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
       <c r="F4" s="13" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="G4" s="28">
         <v>0</v>
@@ -1632,10 +1638,10 @@
         <v>401</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K4" s="26">
         <v>99</v>
@@ -1662,11 +1668,11 @@
         <v>32</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G5" s="28">
         <v>0</v>
@@ -1675,10 +1681,10 @@
         <v>401</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K5" s="26">
         <v>99</v>
@@ -1718,10 +1724,10 @@
         <v>401</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K6" s="26">
         <v>99</v>
@@ -1761,10 +1767,10 @@
         <v>422</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K7" s="29">
         <v>90</v>
@@ -1793,7 +1799,7 @@
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
       <c r="F8" s="29" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="G8" s="30">
         <v>0</v>
@@ -1802,10 +1808,10 @@
         <v>401</v>
       </c>
       <c r="I8" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K8" s="29">
         <v>90</v>
@@ -1832,11 +1838,11 @@
         <v>32</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9" s="30">
         <v>0</v>
@@ -1845,10 +1851,10 @@
         <v>401</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K9" s="29">
         <v>90</v>
@@ -1929,10 +1935,10 @@
         <v>422</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K11" s="26">
         <v>80</v>
@@ -1948,7 +1954,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>46</v>
       </c>
@@ -1961,7 +1967,7 @@
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
       <c r="F12" s="13" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="G12" s="28">
         <v>0</v>
@@ -1970,10 +1976,10 @@
         <v>401</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K12" s="26">
         <v>80</v>
@@ -2000,11 +2006,11 @@
         <v>32</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="28">
         <v>0</v>
@@ -2013,10 +2019,10 @@
         <v>401</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K13" s="26">
         <v>80</v>
@@ -2097,10 +2103,10 @@
         <v>422</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K15" s="29">
         <v>10</v>
@@ -2140,10 +2146,10 @@
         <v>422</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K16" s="29">
         <v>20</v>
@@ -2202,7 +2208,7 @@
     </row>
     <row r="18" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" s="26">
         <v>16</v>
@@ -2211,7 +2217,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="13" t="s">
@@ -2224,7 +2230,7 @@
         <v>422</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="26">
@@ -2243,7 +2249,7 @@
     </row>
     <row r="19" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="26">
         <v>17</v>
@@ -2252,7 +2258,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="13" t="s">
@@ -2265,7 +2271,7 @@
         <v>422</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="26">
@@ -2284,7 +2290,7 @@
     </row>
     <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="26">
         <v>18</v>
@@ -2293,7 +2299,7 @@
         <v>32</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20" s="16" t="s">
@@ -2306,7 +2312,7 @@
         <v>422</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="26">
@@ -2325,7 +2331,7 @@
     </row>
     <row r="21" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B21" s="26">
         <v>19</v>
@@ -2334,11 +2340,11 @@
         <v>32</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" s="26"/>
       <c r="F21" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G21" s="28">
         <v>5</v>
@@ -2347,10 +2353,10 @@
         <v>401</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K21" s="26">
         <v>10</v>
@@ -2368,7 +2374,7 @@
     </row>
     <row r="22" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B22" s="26">
         <v>20</v>
@@ -2377,11 +2383,11 @@
         <v>32</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22" s="26"/>
       <c r="F22" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G22" s="28">
         <v>3</v>
@@ -2390,10 +2396,10 @@
         <v>401</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K22" s="26">
         <v>10</v>
@@ -2411,7 +2417,7 @@
     </row>
     <row r="23" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B23" s="26">
         <v>21</v>
@@ -2420,11 +2426,11 @@
         <v>32</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G23" s="28">
         <v>0</v>
@@ -2470,7 +2476,7 @@
         <v>422</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J24" s="20"/>
       <c r="K24" s="29">
@@ -2487,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>34</v>
       </c>
@@ -2500,35 +2506,33 @@
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="20" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="G25" s="30">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H25" s="30">
         <v>401</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="K25" s="29">
         <v>30</v>
       </c>
-      <c r="L25" s="29">
-        <v>90</v>
+      <c r="L25" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="M25" s="21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(L25,State!$A$3:$B$9,2,FALSE),"")</f>
-        <v xml:space="preserve">Blocked </v>
-      </c>
-      <c r="N25" s="31" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+      <c r="N25" s="32"/>
+    </row>
+    <row r="26" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>34</v>
       </c>
@@ -2541,35 +2545,35 @@
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="20" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="G26" s="30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H26" s="30">
         <v>401</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="K26" s="29">
         <v>30</v>
       </c>
-      <c r="L26" s="29" t="s">
-        <v>51</v>
+      <c r="L26" s="29">
+        <v>90</v>
       </c>
       <c r="M26" s="21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(L26,State!$A$3:$B$9,2,FALSE),"")</f>
-        <v/>
+        <v xml:space="preserve">Blocked </v>
       </c>
       <c r="N26" s="31" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>34</v>
       </c>
@@ -2582,18 +2586,20 @@
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="20" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="G27" s="30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27" s="30">
-        <v>200</v>
+        <v>401</v>
       </c>
       <c r="I27" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="J27" s="20"/>
+        <v>72</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>90</v>
+      </c>
       <c r="K27" s="29">
         <v>30</v>
       </c>
@@ -2604,52 +2610,50 @@
         <f>_xlfn.IFNA(VLOOKUP(L27,State!$A$3:$B$9,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="N27" s="32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="26">
+      <c r="N27" s="31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="29">
         <v>26</v>
       </c>
-      <c r="C28" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="28">
-        <v>0</v>
-      </c>
-      <c r="H28" s="28">
-        <v>422</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="J28" s="16"/>
-      <c r="K28" s="26">
-        <v>10</v>
-      </c>
-      <c r="L28" s="26" t="s">
+      <c r="C28" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="30">
+        <v>0</v>
+      </c>
+      <c r="H28" s="30">
+        <v>200</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="J28" s="20"/>
+      <c r="K28" s="29">
+        <v>30</v>
+      </c>
+      <c r="L28" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="M28" s="17" t="str">
+      <c r="M28" s="21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(L28,State!$A$3:$B$9,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="N28" s="27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="N28" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>50</v>
       </c>
@@ -2664,30 +2668,30 @@
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29" s="28">
         <v>0</v>
       </c>
       <c r="H29" s="28">
-        <v>200</v>
+        <v>422</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="26">
-        <v>20</v>
-      </c>
-      <c r="L29" s="26">
         <v>10</v>
+      </c>
+      <c r="L29" s="26" t="s">
+        <v>51</v>
       </c>
       <c r="M29" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(L29,State!$A$3:$B$9,2,FALSE),"")</f>
-        <v>Inactive</v>
+        <v/>
       </c>
       <c r="N29" s="27" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -2718,7 +2722,7 @@
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="26">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L30" s="26">
         <v>10</v>
@@ -2728,6 +2732,47 @@
         <v>Inactive</v>
       </c>
       <c r="N30" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="26">
+        <v>29</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="28">
+        <v>0</v>
+      </c>
+      <c r="H31" s="28">
+        <v>200</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="16"/>
+      <c r="K31" s="26">
+        <v>30</v>
+      </c>
+      <c r="L31" s="26">
+        <v>10</v>
+      </c>
+      <c r="M31" s="17" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(L31,State!$A$3:$B$9,2,FALSE),"")</f>
+        <v>Inactive</v>
+      </c>
+      <c r="N31" s="27" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Login status added and logout implemented
</commit_message>
<xml_diff>
--- a/documentation/Automatic_tests.xlsx
+++ b/documentation/Automatic_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0054B3E8-BFB7-5B44-BE04-08E24D50939F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7916AAD3-9E67-9247-90FD-5E0C4C77CFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1100" windowWidth="27640" windowHeight="19300" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="91">
   <si>
     <t>-</t>
   </si>
@@ -1544,8 +1544,8 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2611,21 +2611,23 @@
         <v>0</v>
       </c>
       <c r="H26" s="42">
-        <v>200</v>
+        <v>403</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="J26" s="19"/>
+        <v>71</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>90</v>
+      </c>
       <c r="K26" s="28">
         <v>20</v>
       </c>
       <c r="L26" s="28">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M26" s="20" t="str">
         <f>_xlfn.IFNA(VLOOKUP(L26,State!$A$3:$B$9,2,FALSE),"")</f>
-        <v>Active</v>
+        <v>Acknowledged</v>
       </c>
       <c r="N26" s="30" t="s">
         <v>0</v>
@@ -2820,11 +2822,11 @@
         <v>30</v>
       </c>
       <c r="L31" s="28">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M31" s="20" t="str">
         <f>_xlfn.IFNA(VLOOKUP(L31,State!$A$3:$B$9,2,FALSE),"")</f>
-        <v>Active</v>
+        <v/>
       </c>
       <c r="N31" s="31" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Logout test added for TDD
</commit_message>
<xml_diff>
--- a/documentation/Automatic_tests.xlsx
+++ b/documentation/Automatic_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7916AAD3-9E67-9247-90FD-5E0C4C77CFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69B2CA0-E5DF-8C47-9332-349371207080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1100" windowWidth="27640" windowHeight="19300" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="93">
   <si>
     <t>-</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>The user has not the right status.</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>logout</t>
   </si>
 </sst>
 </file>
@@ -1541,11 +1547,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DB7162-4CDB-1E49-A9D6-A74F09DB89DA}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2996,8 +3002,207 @@
         <v>40</v>
       </c>
     </row>
+    <row r="36" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="28">
+        <v>34</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="29">
+        <v>0</v>
+      </c>
+      <c r="H36" s="42">
+        <v>422</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J36" s="19"/>
+      <c r="K36" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="M36" s="20" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(L36,State!$A$3:$B$9,2,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="N36" s="30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="28">
+        <v>35</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="29">
+        <v>0</v>
+      </c>
+      <c r="H37" s="42">
+        <v>403</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="K37" s="28">
+        <v>10</v>
+      </c>
+      <c r="L37" s="28">
+        <v>10</v>
+      </c>
+      <c r="M37" s="20" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(L37,State!$A$3:$B$9,2,FALSE),"")</f>
+        <v>Inactive</v>
+      </c>
+      <c r="N37" s="30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="28">
+        <v>36</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38" s="29">
+        <v>0</v>
+      </c>
+      <c r="H38" s="42">
+        <v>403</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="K38" s="28">
+        <v>20</v>
+      </c>
+      <c r="L38" s="28">
+        <v>20</v>
+      </c>
+      <c r="M38" s="20" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(L38,State!$A$3:$B$9,2,FALSE),"")</f>
+        <v>Acknowledged</v>
+      </c>
+      <c r="N38" s="30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="28">
+        <v>37</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G39" s="29">
+        <v>0</v>
+      </c>
+      <c r="H39" s="42">
+        <v>403</v>
+      </c>
+      <c r="I39" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="K39" s="28">
+        <v>30</v>
+      </c>
+      <c r="L39" s="28">
+        <v>30</v>
+      </c>
+      <c r="M39" s="20" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(L39,State!$A$3:$B$9,2,FALSE),"")</f>
+        <v>Active</v>
+      </c>
+      <c r="N39" s="30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="28">
+        <v>38</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G40" s="29">
+        <v>0</v>
+      </c>
+      <c r="H40" s="42">
+        <v>200</v>
+      </c>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="28">
+        <v>40</v>
+      </c>
+      <c r="L40" s="28">
+        <v>30</v>
+      </c>
+      <c r="M40" s="20" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(L40,State!$A$3:$B$9,2,FALSE),"")</f>
+        <v>Active</v>
+      </c>
+      <c r="N40" s="30" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H3:H35">
+  <conditionalFormatting sqref="H3:H40">
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>$H3=403</formula>
     </cfRule>
@@ -3011,7 +3216,7 @@
       <formula>$H3=401</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L35">
+  <conditionalFormatting sqref="L3:L40">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>$K3&lt;&gt;$L3</formula>
     </cfRule>

</xml_diff>

<commit_message>
Automatic login possibility also with test endpoint
</commit_message>
<xml_diff>
--- a/documentation/Automatic_tests.xlsx
+++ b/documentation/Automatic_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Peter/Development/Python/Fishing/V2/1_Preparation/fishing/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69B2CA0-E5DF-8C47-9332-349371207080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE439990-CF8F-644F-A790-6CEE84887DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="1100" windowWidth="27640" windowHeight="19300" activeTab="2" xr2:uid="{CB59B4E2-ABBB-9640-84E4-2E991D1E5FE4}"/>
   </bookViews>
@@ -292,9 +292,6 @@
     <t>email, password</t>
   </si>
   <si>
-    <t>{"access_token": "*STRING", "token_type": "Bearer"}</t>
-  </si>
-  <si>
     <t>Invalid login attempt.</t>
   </si>
   <si>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>logout</t>
+  </si>
+  <si>
+    <t>{"token": "*STRING", "token_type": "Bearer"}</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1648,7 +1648,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="27">
         <v>0</v>
@@ -1818,7 +1818,7 @@
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="29">
         <v>0</v>
@@ -1986,7 +1986,7 @@
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="27">
         <v>0</v>
@@ -2295,7 +2295,7 @@
         <v>71</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K18" s="25">
         <v>10</v>
@@ -2379,7 +2379,7 @@
         <v>71</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K20" s="25">
         <v>20</v>
@@ -2570,7 +2570,7 @@
       <c r="D25" s="28"/>
       <c r="E25" s="28"/>
       <c r="F25" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G25" s="29">
         <v>0</v>
@@ -2582,7 +2582,7 @@
         <v>71</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K25" s="28">
         <v>10</v>
@@ -2611,7 +2611,7 @@
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
       <c r="F26" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G26" s="29">
         <v>0</v>
@@ -2623,7 +2623,7 @@
         <v>71</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K26" s="28">
         <v>20</v>
@@ -2652,7 +2652,7 @@
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
       <c r="F27" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27" s="29">
         <v>0</v>
@@ -2664,7 +2664,7 @@
         <v>71</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K27" s="28">
         <v>30</v>
@@ -2691,7 +2691,7 @@
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
       <c r="F28" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G28" s="29">
         <v>5</v>
@@ -2732,7 +2732,7 @@
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G29" s="29">
         <v>3</v>
@@ -2744,7 +2744,7 @@
         <v>71</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K29" s="28">
         <v>30</v>
@@ -2812,7 +2812,7 @@
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G31" s="29">
         <v>0</v>
@@ -2821,7 +2821,7 @@
         <v>200</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="J31" s="19"/>
       <c r="K31" s="28">
@@ -3004,13 +3004,13 @@
     </row>
     <row r="36" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36" s="28">
         <v>34</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
@@ -3043,13 +3043,13 @@
     </row>
     <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" s="28">
         <v>35</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
@@ -3066,7 +3066,7 @@
         <v>71</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K37" s="28">
         <v>10</v>
@@ -3084,13 +3084,13 @@
     </row>
     <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" s="28">
         <v>36</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" s="28"/>
       <c r="E38" s="28"/>
@@ -3107,7 +3107,7 @@
         <v>71</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K38" s="28">
         <v>20</v>
@@ -3125,13 +3125,13 @@
     </row>
     <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" s="28">
         <v>37</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D39" s="28"/>
       <c r="E39" s="28"/>
@@ -3148,7 +3148,7 @@
         <v>71</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K39" s="28">
         <v>30</v>
@@ -3166,13 +3166,13 @@
     </row>
     <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="28">
         <v>38</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40" s="28"/>
       <c r="E40" s="28"/>

</xml_diff>